<commit_message>
Commit prior to dynamic steps.
</commit_message>
<xml_diff>
--- a/xlsx_SSC_Simulation.xlsx
+++ b/xlsx_SSC_Simulation.xlsx
@@ -14,35 +14,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="32">
   <si>
     <t>x</t>
   </si>
   <si>
+    <t>Scott</t>
+  </si>
+  <si>
+    <t>Sally</t>
+  </si>
+  <si>
+    <t>Tomas</t>
+  </si>
+  <si>
+    <t>Jim</t>
+  </si>
+  <si>
     <t>Lillian</t>
   </si>
   <si>
+    <t>Joe</t>
+  </si>
+  <si>
     <t>Diane</t>
   </si>
   <si>
-    <t>Lynn</t>
-  </si>
-  <si>
-    <t>Jim</t>
-  </si>
-  <si>
-    <t>Sally</t>
-  </si>
-  <si>
-    <t>Scott</t>
-  </si>
-  <si>
-    <t>Tomas</t>
-  </si>
-  <si>
-    <t>Joe</t>
-  </si>
-  <si>
     <t xml:space="preserve">Name: </t>
   </si>
   <si>
@@ -67,58 +64,52 @@
     <t xml:space="preserve">Potential Con: </t>
   </si>
   <si>
-    <t>12,14</t>
-  </si>
-  <si>
-    <t>potential_host</t>
+    <t>6,13</t>
+  </si>
+  <si>
+    <t>resting</t>
   </si>
   <si>
     <t>Verizon</t>
   </si>
   <si>
-    <t>5,6</t>
+    <t>12,9</t>
+  </si>
+  <si>
+    <t>potential_client</t>
+  </si>
+  <si>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>5,8</t>
   </si>
   <si>
     <t>client</t>
   </si>
   <si>
-    <t>5,12</t>
-  </si>
-  <si>
-    <t>resting</t>
-  </si>
-  <si>
-    <t>Sprint</t>
-  </si>
-  <si>
-    <t>14,6</t>
+    <t>ATnT</t>
+  </si>
+  <si>
+    <t>6,5</t>
+  </si>
+  <si>
+    <t>7,13</t>
   </si>
   <si>
     <t>host</t>
   </si>
   <si>
-    <t>ATnT</t>
-  </si>
-  <si>
-    <t>9,4</t>
-  </si>
-  <si>
-    <t>potential_client</t>
-  </si>
-  <si>
-    <t>12,15</t>
-  </si>
-  <si>
-    <t>1,14</t>
-  </si>
-  <si>
-    <t>11,1</t>
-  </si>
-  <si>
-    <t>8,7</t>
-  </si>
-  <si>
-    <t>0,6</t>
+    <t>3,5</t>
+  </si>
+  <si>
+    <t>8,14</t>
+  </si>
+  <si>
+    <t>7,10</t>
+  </si>
+  <si>
+    <t>3,4</t>
   </si>
 </sst>
 </file>
@@ -450,7 +441,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P29"/>
+  <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -541,7 +532,7 @@
         <v>0</v>
       </c>
       <c r="L2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2" t="s">
         <v>0</v>
@@ -667,7 +658,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" t="s">
         <v>0</v>
@@ -685,7 +676,7 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K5" t="s">
         <v>0</v>
@@ -717,7 +708,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E6" t="s">
         <v>0</v>
@@ -726,7 +717,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H6" t="s">
         <v>0</v>
@@ -758,7 +749,7 @@
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
@@ -773,7 +764,7 @@
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G7" t="s">
         <v>0</v>
@@ -800,7 +791,7 @@
         <v>0</v>
       </c>
       <c r="O7" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="P7" t="s">
         <v>0</v>
@@ -832,7 +823,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J8" t="s">
         <v>0</v>
@@ -873,7 +864,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G9" t="s">
         <v>0</v>
@@ -944,7 +935,7 @@
         <v>0</v>
       </c>
       <c r="M10" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N10" t="s">
         <v>0</v>
@@ -979,7 +970,7 @@
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I11" t="s">
         <v>0</v>
@@ -1073,7 +1064,7 @@
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G13" t="s">
         <v>0</v>
@@ -1126,10 +1117,10 @@
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H14" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I14" t="s">
         <v>0</v>
@@ -1161,7 +1152,7 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
@@ -1182,7 +1173,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" t="s">
         <v>0</v>
@@ -1194,7 +1185,7 @@
         <v>0</v>
       </c>
       <c r="M15" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="N15" t="s">
         <v>0</v>
@@ -1244,7 +1235,7 @@
         <v>0</v>
       </c>
       <c r="M16" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N16" t="s">
         <v>0</v>
@@ -1256,67 +1247,64 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" t="s">
         <v>7</v>
       </c>
-      <c r="E17" t="s">
+      <c r="G17" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" t="s">
+        <v>1</v>
+      </c>
+      <c r="I17" t="s">
         <v>5</v>
       </c>
-      <c r="F17" t="s">
-        <v>2</v>
-      </c>
-      <c r="G17" t="s">
-        <v>5</v>
-      </c>
-      <c r="H17" t="s">
-        <v>6</v>
-      </c>
-      <c r="I17" t="s">
-        <v>1</v>
-      </c>
       <c r="J17" t="s">
-        <v>6</v>
-      </c>
-      <c r="K17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18" t="s">
+      <c r="G18" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
         <v>10</v>
       </c>
-      <c r="C18" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>6</v>
-      </c>
-      <c r="I18" t="s">
-        <v>4</v>
-      </c>
-      <c r="J18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="A19" t="s">
-        <v>11</v>
-      </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D19" t="s">
         <v>22</v>
@@ -1325,118 +1313,109 @@
         <v>25</v>
       </c>
       <c r="F19" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" t="s">
         <v>28</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
+        <v>29</v>
+      </c>
+      <c r="I19" t="s">
         <v>30</v>
       </c>
-      <c r="H19" t="s">
+      <c r="J19" t="s">
         <v>31</v>
       </c>
-      <c r="I19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J19" t="s">
-        <v>33</v>
-      </c>
-      <c r="K19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D20" t="s">
         <v>23</v>
       </c>
       <c r="E20" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="F20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H20" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" t="s">
         <v>18</v>
       </c>
-      <c r="H20" t="s">
-        <v>18</v>
-      </c>
-      <c r="I20" t="s">
-        <v>26</v>
-      </c>
-      <c r="J20" t="s">
+      <c r="C21" t="s">
         <v>21</v>
-      </c>
-      <c r="K20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" t="s">
-        <v>19</v>
       </c>
       <c r="D21" t="s">
         <v>24</v>
       </c>
       <c r="E21" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F21" t="s">
         <v>24</v>
       </c>
       <c r="G21" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="H21" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" t="s">
         <v>24</v>
       </c>
-      <c r="I21" t="s">
-        <v>27</v>
-      </c>
       <c r="J21" t="s">
-        <v>24</v>
-      </c>
-      <c r="K21" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
       <c r="D22">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E22">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22">
         <v>1</v>
       </c>
       <c r="H22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22">
         <v>4</v>
@@ -1444,178 +1423,229 @@
       <c r="J22">
         <v>0</v>
       </c>
-      <c r="K22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B23">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C23">
         <v>4</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="H23">
+        <v>4</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" t="s">
         <v>3</v>
       </c>
-      <c r="H23">
-        <v>2</v>
-      </c>
-      <c r="I23">
+      <c r="H24" t="s">
+        <v>6</v>
+      </c>
+      <c r="I24" t="s">
+        <v>6</v>
+      </c>
+      <c r="J24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="B25" t="s">
         <v>4</v>
       </c>
-      <c r="J23">
-        <v>1</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="A24" t="s">
-        <v>16</v>
-      </c>
-      <c r="B24" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>4</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" t="s">
         <v>4</v>
       </c>
-      <c r="E24" t="s">
+      <c r="G25" t="s">
+        <v>2</v>
+      </c>
+      <c r="H25" t="s">
+        <v>4</v>
+      </c>
+      <c r="I25" t="s">
+        <v>4</v>
+      </c>
+      <c r="J25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26" t="s">
+        <v>2</v>
+      </c>
+      <c r="H26" t="s">
+        <v>3</v>
+      </c>
+      <c r="I26" t="s">
+        <v>3</v>
+      </c>
+      <c r="J26" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" t="s">
         <v>5</v>
       </c>
-      <c r="F24" t="s">
-        <v>4</v>
-      </c>
-      <c r="G24" t="s">
-        <v>8</v>
-      </c>
-      <c r="H24" t="s">
+      <c r="H27" t="s">
         <v>7</v>
       </c>
-      <c r="I24" t="s">
-        <v>4</v>
-      </c>
-      <c r="J24" t="s">
-        <v>4</v>
-      </c>
-      <c r="K24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="B25" t="s">
+      <c r="I27" t="s">
+        <v>2</v>
+      </c>
+      <c r="J27" t="s">
         <v>5</v>
       </c>
-      <c r="C25" t="s">
+    </row>
+    <row r="28" spans="1:10">
+      <c r="B28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" t="s">
+        <v>5</v>
+      </c>
+      <c r="F28" t="s">
+        <v>1</v>
+      </c>
+      <c r="G28" t="s">
+        <v>1</v>
+      </c>
+      <c r="H28" t="s">
+        <v>1</v>
+      </c>
+      <c r="I28" t="s">
         <v>7</v>
       </c>
-      <c r="D25" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" t="s">
-        <v>2</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="J28" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="B29" t="s">
         <v>5</v>
       </c>
-      <c r="G25" t="s">
+      <c r="C29" t="s">
         <v>5</v>
       </c>
-      <c r="H25" t="s">
-        <v>6</v>
-      </c>
-      <c r="I25" t="s">
+      <c r="D29" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" t="s">
         <v>5</v>
       </c>
-      <c r="J25" t="s">
-        <v>7</v>
-      </c>
-      <c r="K25" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11">
-      <c r="C26" t="s">
-        <v>2</v>
-      </c>
-      <c r="D26" t="s">
-        <v>6</v>
-      </c>
-      <c r="E26" t="s">
-        <v>1</v>
-      </c>
-      <c r="F26" t="s">
-        <v>2</v>
-      </c>
-      <c r="I26" t="s">
-        <v>2</v>
-      </c>
-      <c r="J26" t="s">
+      <c r="H29" t="s">
         <v>5</v>
       </c>
-      <c r="K26" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="C27" t="s">
-        <v>1</v>
-      </c>
-      <c r="D27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E27" t="s">
-        <v>6</v>
-      </c>
-      <c r="F27" t="s">
-        <v>1</v>
-      </c>
-      <c r="I27" t="s">
-        <v>1</v>
-      </c>
-      <c r="J27" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="C28" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" t="s">
-        <v>3</v>
-      </c>
-      <c r="F28" t="s">
-        <v>6</v>
-      </c>
-      <c r="I28" t="s">
-        <v>6</v>
-      </c>
-      <c r="J28" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
-      <c r="C29" t="s">
-        <v>3</v>
-      </c>
-      <c r="J29" t="s">
-        <v>6</v>
+      <c r="I29" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="D30" t="s">
+        <v>5</v>
+      </c>
+      <c r="I30" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="D31" t="s">
+        <v>1</v>
+      </c>
+      <c r="I31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="I32" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>